<commit_message>
add message.html & try/except for inserting from excel to database
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t xml:space="preserve">Row</t>
   </si>
@@ -75,6 +75,39 @@
   </si>
   <si>
     <t xml:space="preserve">JJ3000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amo hasan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alaki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in chie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amo mamad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SH80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SH100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dolaki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS1500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS1600</t>
   </si>
   <si>
     <t xml:space="preserve">Faulty</t>
@@ -100,7 +133,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -128,11 +161,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -196,7 +224,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -277,13 +305,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.26"/>
@@ -388,6 +416,66 @@
         <v>17</v>
       </c>
       <c r="F5" s="2" t="n">
+        <v>41092</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>34234</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="2" t="n">
         <v>41092</v>
       </c>
     </row>
@@ -409,30 +497,30 @@
   </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -442,7 +530,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>